<commit_message>
feat(utils): Parse number format for output Cell captures Excel number format on load Excel stores output format in formulae property utils methods and tests to apply format
</commit_message>
<xml_diff>
--- a/examples/angles.xlsx
+++ b/examples/angles.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,6 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Mark\dev\ExCell\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD4B1C5-8EB3-4AE7-AB23-8E7D07F25ABD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21915" windowHeight="25635" xr2:uid="{16E37FAE-338D-49C7-8F8E-A92E5B2567EB}"/>
   </bookViews>
@@ -107,6 +108,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,8 +153,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,20 +474,20 @@
   <dimension ref="B2:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2">
+      <c r="B2" s="1">
         <v>3</v>
       </c>
       <c r="D2">
         <f>(B2-2)*180</f>
         <v>180</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <f>D2/B2</f>
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
feat(Inputs): Display formatting from Excel sheet
</commit_message>
<xml_diff>
--- a/examples/angles.xlsx
+++ b/examples/angles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Data\Mark\dev\ExCell\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD4B1C5-8EB3-4AE7-AB23-8E7D07F25ABD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B174A08-ABC4-4294-ACE7-F9353ABE0F44}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21915" windowHeight="25635" xr2:uid="{16E37FAE-338D-49C7-8F8E-A92E5B2567EB}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -156,7 +156,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>